<commit_message>
Site updated at 2017-01-05 19:50:28 UTC
</commit_message>
<xml_diff>
--- a/flyers/Agenda_Grimbergen_2017.xlsx
+++ b/flyers/Agenda_Grimbergen_2017.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="23">
   <si>
     <t xml:space="preserve"> Januari 2017</t>
   </si>
@@ -64,10 +64,16 @@
     <t xml:space="preserve">Za</t>
   </si>
   <si>
+    <t xml:space="preserve">Anne-Marie</t>
+  </si>
+  <si>
     <t xml:space="preserve">Taiji</t>
   </si>
   <si>
-    <t xml:space="preserve">Anne-Marie</t>
+    <t xml:space="preserve">Frank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karine</t>
   </si>
   <si>
     <t xml:space="preserve"> April 2017</t>
@@ -224,7 +230,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -281,31 +287,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -396,20 +394,23 @@
   </sheetPr>
   <dimension ref="1:67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A51" colorId="64" zoomScale="110" zoomScaleNormal="125" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I51" activeCellId="0" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="3.36150234741784"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.32394366197183"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="3.28169014084507"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.6150234741784"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.32394366197183"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="0.962441314553991"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="3.03755868544601"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="8.80281690140845"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="1.28169014084507"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="2.96244131455399"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.6150234741784"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.80281690140845"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="1.2018779342723"/>
     <col collapsed="false" hidden="false" max="14" min="13" style="0" width="2.72300469483568"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="8.80281690140845"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.6150234741784"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="8.80281690140845"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.2065727699531"/>
   </cols>
   <sheetData>
@@ -656,10 +657,12 @@
       <c r="H8" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14" t="s">
-        <v>14</v>
+      <c r="I8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="7" t="s">
@@ -668,10 +671,12 @@
       <c r="N8" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="O8" s="15"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14" t="s">
-        <v>14</v>
+      <c r="O8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,10 +727,12 @@
       <c r="H10" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14" t="s">
-        <v>14</v>
+      <c r="I10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="7" t="s">
@@ -734,10 +741,12 @@
       <c r="N10" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14" t="s">
-        <v>14</v>
+      <c r="O10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,10 +756,12 @@
       <c r="B11" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
-        <v>14</v>
+      <c r="C11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="7" t="s">
@@ -790,12 +801,14 @@
       <c r="H12" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>14</v>
+      <c r="I12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L12" s="10"/>
       <c r="M12" s="7" t="s">
@@ -804,12 +817,14 @@
       <c r="N12" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q12" s="14" t="s">
-        <v>14</v>
+      <c r="O12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,10 +834,12 @@
       <c r="B13" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
-        <v>14</v>
+      <c r="C13" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="7" t="s">
@@ -883,12 +900,14 @@
       <c r="B15" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>14</v>
+      <c r="C15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="7" t="s">
@@ -897,10 +916,12 @@
       <c r="H15" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14" t="s">
-        <v>14</v>
+      <c r="I15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L15" s="10"/>
       <c r="M15" s="7" t="s">
@@ -909,10 +930,12 @@
       <c r="N15" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14" t="s">
-        <v>14</v>
+      <c r="O15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -963,10 +986,12 @@
       <c r="H17" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14" t="s">
-        <v>14</v>
+      <c r="I17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="7" t="s">
@@ -975,10 +1000,12 @@
       <c r="N17" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="O17" s="15"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14" t="s">
-        <v>14</v>
+      <c r="O17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -988,10 +1015,12 @@
       <c r="B18" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14" t="s">
-        <v>14</v>
+      <c r="C18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="7" t="s">
@@ -1031,12 +1060,14 @@
       <c r="H19" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="14" t="s">
-        <v>14</v>
+      <c r="I19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="7" t="s">
@@ -1045,14 +1076,14 @@
       <c r="N19" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="O19" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="P19" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q19" s="14" t="s">
-        <v>14</v>
+      <c r="O19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q19" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,10 +1093,12 @@
       <c r="B20" s="8" t="n">
         <v>18</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14" t="s">
-        <v>14</v>
+      <c r="C20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="7" t="s">
@@ -1126,12 +1159,14 @@
       <c r="B22" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>14</v>
+      <c r="C22" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="7" t="s">
@@ -1140,10 +1175,12 @@
       <c r="H22" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14" t="s">
-        <v>14</v>
+      <c r="I22" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L22" s="10"/>
       <c r="M22" s="7" t="s">
@@ -1152,12 +1189,12 @@
       <c r="N22" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="O22" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14" t="s">
-        <v>14</v>
+      <c r="O22" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1208,10 +1245,12 @@
       <c r="H24" s="8" t="n">
         <v>22</v>
       </c>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14" t="s">
-        <v>14</v>
+      <c r="I24" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L24" s="10"/>
       <c r="M24" s="7" t="s">
@@ -1220,12 +1259,12 @@
       <c r="N24" s="8" t="n">
         <v>22</v>
       </c>
-      <c r="O24" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14" t="s">
-        <v>14</v>
+      <c r="O24" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1235,10 +1274,12 @@
       <c r="B25" s="8" t="n">
         <v>23</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14" t="s">
-        <v>14</v>
+      <c r="C25" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="7" t="s">
@@ -1278,12 +1319,14 @@
       <c r="H26" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K26" s="14" t="s">
-        <v>14</v>
+      <c r="I26" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L26" s="10"/>
       <c r="M26" s="7" t="s">
@@ -1292,12 +1335,14 @@
       <c r="N26" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="O26" s="15"/>
-      <c r="P26" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q26" s="14" t="s">
-        <v>14</v>
+      <c r="O26" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q26" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1307,10 +1352,12 @@
       <c r="B27" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14" t="s">
-        <v>14</v>
+      <c r="C27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="7" t="s">
@@ -1371,12 +1418,14 @@
       <c r="B29" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>14</v>
+      <c r="C29" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="7" t="s">
@@ -1453,7 +1502,7 @@
       <c r="N31" s="8" t="n">
         <v>29</v>
       </c>
-      <c r="O31" s="18"/>
+      <c r="O31" s="17"/>
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
     </row>
@@ -1480,7 +1529,7 @@
       <c r="N32" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="O32" s="18"/>
+      <c r="O32" s="17"/>
       <c r="P32" s="12"/>
       <c r="Q32" s="12"/>
     </row>
@@ -1534,7 +1583,7 @@
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="4"/>
@@ -1542,7 +1591,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="2"/>
       <c r="I35" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="4"/>
@@ -1550,7 +1599,7 @@
       <c r="M35" s="1"/>
       <c r="N35" s="2"/>
       <c r="O35" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="P35" s="2"/>
       <c r="Q35" s="4"/>
@@ -1677,10 +1726,10 @@
       <c r="H39" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14" t="s">
-        <v>14</v>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L39" s="10"/>
       <c r="M39" s="7" t="s">
@@ -1793,7 +1842,7 @@
       <c r="B43" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="C43" s="18"/>
+      <c r="C43" s="17"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="5"/>
@@ -1813,12 +1862,12 @@
       <c r="N43" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="O43" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14" t="s">
-        <v>19</v>
+      <c r="O43" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,10 +1887,10 @@
       <c r="H44" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14" t="s">
-        <v>14</v>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L44" s="10"/>
       <c r="M44" s="7" t="s">
@@ -1881,14 +1930,14 @@
       <c r="N45" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="O45" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="P45" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q45" s="14" t="s">
-        <v>20</v>
+      <c r="O45" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P45" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q45" s="15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,10 +1957,10 @@
       <c r="H46" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14" t="s">
-        <v>14</v>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L46" s="10"/>
       <c r="M46" s="7" t="s">
@@ -1972,12 +2021,12 @@
       <c r="H48" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K48" s="14" t="s">
-        <v>14</v>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L48" s="10"/>
       <c r="M48" s="7" t="s">
@@ -1986,10 +2035,10 @@
       <c r="N48" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14" t="s">
-        <v>14</v>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1999,7 +2048,7 @@
       <c r="B49" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="C49" s="18"/>
+      <c r="C49" s="17"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="5"/>
@@ -2030,7 +2079,7 @@
       <c r="B50" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="C50" s="18"/>
+      <c r="C50" s="17"/>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="5"/>
@@ -2050,10 +2099,10 @@
       <c r="N50" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
-      <c r="Q50" s="14" t="s">
-        <v>14</v>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2073,12 +2122,12 @@
       <c r="H51" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="I51" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14" t="s">
-        <v>14</v>
+      <c r="I51" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L51" s="10"/>
       <c r="M51" s="7" t="s">
@@ -2118,12 +2167,12 @@
       <c r="N52" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="O52" s="15"/>
-      <c r="P52" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q52" s="14" t="s">
-        <v>14</v>
+      <c r="O52" s="18"/>
+      <c r="P52" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q52" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,12 +2192,12 @@
       <c r="H53" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="I53" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14" t="s">
-        <v>14</v>
+      <c r="I53" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L53" s="10"/>
       <c r="M53" s="7" t="s">
@@ -2178,7 +2227,7 @@
       <c r="H54" s="8" t="n">
         <v>18</v>
       </c>
-      <c r="I54" s="20"/>
+      <c r="I54" s="8"/>
       <c r="J54" s="16"/>
       <c r="K54" s="16"/>
       <c r="L54" s="10"/>
@@ -2199,10 +2248,10 @@
       <c r="B55" s="8" t="n">
         <v>19</v>
       </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14" t="s">
-        <v>14</v>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="7" t="s">
@@ -2211,14 +2260,14 @@
       <c r="H55" s="8" t="n">
         <v>19</v>
       </c>
-      <c r="I55" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="J55" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K55" s="14" t="s">
-        <v>14</v>
+      <c r="I55" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K55" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L55" s="10"/>
       <c r="M55" s="7" t="s">
@@ -2227,10 +2276,10 @@
       <c r="N55" s="8" t="n">
         <v>19</v>
       </c>
-      <c r="O55" s="14"/>
-      <c r="P55" s="14"/>
-      <c r="Q55" s="14" t="s">
-        <v>14</v>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2271,12 +2320,12 @@
       <c r="B57" s="8" t="n">
         <v>21</v>
       </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E57" s="14" t="s">
-        <v>14</v>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="7" t="s">
@@ -2285,7 +2334,7 @@
       <c r="H57" s="8" t="n">
         <v>21</v>
       </c>
-      <c r="I57" s="13"/>
+      <c r="I57" s="11"/>
       <c r="J57" s="11"/>
       <c r="K57" s="11"/>
       <c r="L57" s="10"/>
@@ -2295,10 +2344,10 @@
       <c r="N57" s="8" t="n">
         <v>21</v>
       </c>
-      <c r="O57" s="14"/>
-      <c r="P57" s="14"/>
-      <c r="Q57" s="14" t="s">
-        <v>14</v>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
+      <c r="Q57" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2318,12 +2367,12 @@
       <c r="H58" s="8" t="n">
         <v>22</v>
       </c>
-      <c r="I58" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14" t="s">
-        <v>14</v>
+      <c r="I58" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L58" s="10"/>
       <c r="M58" s="7" t="s">
@@ -2363,12 +2412,12 @@
       <c r="N59" s="8" t="n">
         <v>23</v>
       </c>
-      <c r="O59" s="14"/>
-      <c r="P59" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q59" s="14" t="s">
-        <v>14</v>
+      <c r="O59" s="15"/>
+      <c r="P59" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q59" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2378,10 +2427,10 @@
       <c r="B60" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14" t="s">
-        <v>14</v>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="7" t="s">
@@ -2390,12 +2439,12 @@
       <c r="H60" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="I60" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14" t="s">
-        <v>14</v>
+      <c r="I60" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="L60" s="10"/>
       <c r="M60" s="7" t="s">
@@ -2446,10 +2495,10 @@
       <c r="B62" s="8" t="n">
         <v>26</v>
       </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14" t="s">
-        <v>14</v>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="7" t="s">
@@ -2458,7 +2507,7 @@
       <c r="H62" s="8" t="n">
         <v>26</v>
       </c>
-      <c r="I62" s="18"/>
+      <c r="I62" s="17"/>
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
       <c r="L62" s="10"/>
@@ -2468,10 +2517,10 @@
       <c r="N62" s="8" t="n">
         <v>26</v>
       </c>
-      <c r="O62" s="14"/>
-      <c r="P62" s="14"/>
-      <c r="Q62" s="14" t="s">
-        <v>14</v>
+      <c r="O62" s="15"/>
+      <c r="P62" s="15"/>
+      <c r="Q62" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2512,12 +2561,12 @@
       <c r="B64" s="8" t="n">
         <v>28</v>
       </c>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E64" s="14" t="s">
-        <v>14</v>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="7" t="s">
@@ -2536,10 +2585,10 @@
       <c r="N64" s="8" t="n">
         <v>28</v>
       </c>
-      <c r="O64" s="14"/>
-      <c r="P64" s="14"/>
-      <c r="Q64" s="14" t="s">
-        <v>14</v>
+      <c r="O64" s="15"/>
+      <c r="P64" s="15"/>
+      <c r="Q64" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2600,12 +2649,12 @@
       <c r="N66" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="O66" s="14"/>
-      <c r="P66" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q66" s="14" t="s">
-        <v>14</v>
+      <c r="O66" s="15"/>
+      <c r="P66" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q66" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2614,7 +2663,7 @@
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
-      <c r="F67" s="21"/>
+      <c r="F67" s="19"/>
       <c r="G67" s="7" t="s">
         <v>8</v>
       </c>
@@ -2624,7 +2673,7 @@
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
-      <c r="L67" s="22"/>
+      <c r="L67" s="20"/>
       <c r="M67" s="7"/>
       <c r="N67" s="8"/>
       <c r="O67" s="9"/>
@@ -2634,7 +2683,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.0784722222222222" right="0.0784722222222222" top="0.0784722222222222" bottom="0.0784722222222222" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="82" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="83" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>